<commit_message>
update manual check repos
</commit_message>
<xml_diff>
--- a/data_collection/gui_repos.xlsx
+++ b/data_collection/gui_repos.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3035" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3034" uniqueCount="542">
   <si>
     <t xml:space="preserve">repository</t>
   </si>
@@ -1742,7 +1742,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1760,10 +1760,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1791,7 +1787,7 @@
   <dimension ref="A1:A503"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B59:D59 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4329,8 +4325,8 @@
   </sheetPr>
   <dimension ref="A1:C503"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A434" activeCellId="0" sqref="A434"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A156" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B201" activeCellId="1" sqref="B59:D59 B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6533,7 +6529,7 @@
         <v>230</v>
       </c>
       <c r="B200" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>505</v>
@@ -9888,18 +9884,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59:D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="15.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9920,317 +9916,815 @@
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="B4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>70</v>
       </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>75</v>
       </c>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>96</v>
       </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>99</v>
       </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>100</v>
       </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>121</v>
       </c>
+      <c r="B12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>123</v>
       </c>
+      <c r="B13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>136</v>
       </c>
+      <c r="B14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>148</v>
       </c>
+      <c r="B15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>169</v>
       </c>
+      <c r="B16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>181</v>
       </c>
+      <c r="B17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>183</v>
       </c>
+      <c r="B18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>192</v>
       </c>
+      <c r="B19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>204</v>
       </c>
+      <c r="B20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>210</v>
       </c>
+      <c r="B21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>211</v>
       </c>
+      <c r="B22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>229</v>
       </c>
+      <c r="B23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>237</v>
+        <v>243</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>243</v>
+        <v>254</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>254</v>
+        <v>262</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>262</v>
+        <v>288</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>288</v>
+        <v>303</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>307</v>
+        <v>324</v>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>325</v>
+        <v>347</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>347</v>
+        <v>385</v>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>385</v>
+        <v>397</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>397</v>
+        <v>410</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>410</v>
+        <v>415</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
+      </c>
+      <c r="B42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>420</v>
+        <v>432</v>
+      </c>
+      <c r="B43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>432</v>
+        <v>435</v>
+      </c>
+      <c r="B44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>435</v>
+        <v>439</v>
+      </c>
+      <c r="B45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
+      </c>
+      <c r="B46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
+      </c>
+      <c r="B47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
+      </c>
+      <c r="B48" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>447</v>
+        <v>454</v>
+      </c>
+      <c r="B49" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>454</v>
+        <v>459</v>
+      </c>
+      <c r="B50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>459</v>
+        <v>475</v>
+      </c>
+      <c r="B51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>475</v>
+        <v>488</v>
+      </c>
+      <c r="B52" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>488</v>
+        <v>78</v>
+      </c>
+      <c r="B53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>78</v>
+        <v>170</v>
+      </c>
+      <c r="B54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>170</v>
+        <v>214</v>
+      </c>
+      <c r="B55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>214</v>
+        <v>251</v>
+      </c>
+      <c r="B56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>251</v>
+        <v>399</v>
+      </c>
+      <c r="B57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
+      </c>
+      <c r="B58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -10250,7 +10744,7 @@
   <dimension ref="A1:B477"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B59:D59 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14090,7 +14584,7 @@
   <dimension ref="A1:B477"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B59:D59 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17930,7 +18424,7 @@
   <dimension ref="A1:B477"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B59:D59 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21774,10 +22268,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="B59:D59 C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="35.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="16.43"/>
@@ -21886,7 +22380,7 @@
       <c r="A7" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="5" t="b">
+      <c r="B7" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21903,7 +22397,7 @@
       <c r="A8" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B8" s="5" t="b">
+      <c r="B8" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21920,15 +22414,15 @@
       <c r="A9" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B9" s="5" t="b">
+      <c r="B9" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="b">
+      <c r="C9" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D9" s="5" t="b">
+      <c r="D9" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21937,15 +22431,15 @@
       <c r="A10" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B10" s="5" t="b">
+      <c r="B10" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C10" s="5" t="b">
+      <c r="C10" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D10" s="5" t="b">
+      <c r="D10" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21954,15 +22448,15 @@
       <c r="A11" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B11" s="5" t="b">
+      <c r="B11" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="b">
+      <c r="C11" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D11" s="5" t="b">
+      <c r="D11" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21971,15 +22465,15 @@
       <c r="A12" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="B12" s="5" t="b">
+      <c r="B12" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C12" s="5" t="b">
+      <c r="C12" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D12" s="5" t="b">
+      <c r="D12" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21988,15 +22482,15 @@
       <c r="A13" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="B13" s="5" t="b">
+      <c r="B13" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C13" s="5" t="b">
+      <c r="C13" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D13" s="5" t="b">
+      <c r="D13" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22005,15 +22499,15 @@
       <c r="A14" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="B14" s="5" t="b">
+      <c r="B14" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C14" s="5" t="b">
+      <c r="C14" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D14" s="5" t="b">
+      <c r="D14" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22022,7 +22516,7 @@
       <c r="A15" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="B15" s="5" t="b">
+      <c r="B15" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22030,7 +22524,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D15" s="5" t="b">
+      <c r="D15" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22039,7 +22533,7 @@
       <c r="A16" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>541</v>
       </c>
       <c r="C16" s="3" t="s">

</xml_diff>